<commit_message>
Add edition; change creator to author
</commit_message>
<xml_diff>
--- a/doc/PrinttemplateExample.xlsx
+++ b/doc/PrinttemplateExample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emeryr/code/GIT/openn/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5FD270C8-37B3-BC46-8E82-35859D53CB21}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1DF3DD73-52BC-7F48-82DB-5CC054C8B312}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19940" yWindow="460" windowWidth="19960" windowHeight="22580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
     <author>Emery, Doug</author>
   </authors>
   <commentList>
-    <comment ref="B23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -145,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -198,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -241,7 +241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="B30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -295,7 +295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="B31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -339,7 +339,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="B32" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -382,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="B33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -425,7 +425,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B32" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="B34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -488,7 +488,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="B35" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -532,7 +532,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B36" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="B38" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -585,7 +585,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -638,7 +638,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B38" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="B40" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -691,7 +691,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="B41" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -754,7 +754,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B40" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="B42" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -807,7 +807,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B47" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="B49" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -860,7 +860,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B48" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="B50" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -931,7 +931,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B49" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="B51" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -984,7 +984,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B54" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="B56" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -1047,7 +1047,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B55" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="B57" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -1063,7 +1063,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B60" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="B62" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -1116,7 +1116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B63" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
+    <comment ref="B65" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -1179,7 +1179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A66" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+    <comment ref="A68" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -1203,7 +1203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B69" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
+    <comment ref="B71" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
       <text>
         <r>
           <rPr>
@@ -1266,7 +1266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B70" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
+    <comment ref="B72" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
       <text>
         <r>
           <rPr>
@@ -1282,7 +1282,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B79" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
+    <comment ref="B81" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
       <text>
         <r>
           <rPr>
@@ -1427,7 +1427,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3960" uniqueCount="3825">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3969" uniqueCount="3831">
   <si>
     <t>1r</t>
   </si>
@@ -12902,13 +12902,31 @@
   </si>
   <si>
     <t>Following fields are publication info should these be treated as a single repeatable unit?</t>
+  </si>
+  <si>
+    <t>fileDesc/publicationStmt/publisher</t>
+  </si>
+  <si>
+    <t>Metadata Publisher</t>
+  </si>
+  <si>
+    <t>We need a value for the TEI publisher; is it the Holding institution?</t>
+  </si>
+  <si>
+    <t>Edition</t>
+  </si>
+  <si>
+    <t>6/12/2018 Added</t>
+  </si>
+  <si>
+    <t>sourceDesc/biblStruct/monogr/edition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -13071,8 +13089,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -13127,6 +13151,12 @@
         <bgColor rgb="FFDDD9C3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -13148,7 +13178,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -13308,6 +13338,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -13627,13 +13666,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA1007"/>
+  <dimension ref="A1:AA1009"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D47" sqref="D47"/>
+      <selection pane="bottomRight" activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -14287,57 +14326,55 @@
       <c r="Z18" s="15"/>
       <c r="AA18" s="15"/>
     </row>
-    <row r="19" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A19" s="30" t="s">
-        <v>3771</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>307</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="16" t="s">
-        <v>3795</v>
-      </c>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="29"/>
-      <c r="R19" s="29"/>
-      <c r="S19" s="29"/>
-      <c r="T19" s="29"/>
-      <c r="U19" s="29"/>
-      <c r="V19" s="29"/>
-      <c r="W19" s="29"/>
-      <c r="X19" s="29"/>
+    <row r="19" spans="1:27" ht="48">
+      <c r="A19" s="64" t="s">
+        <v>3825</v>
+      </c>
+      <c r="B19" s="65" t="s">
+        <v>3826</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="66" t="s">
+        <v>3827</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
+      <c r="W19" s="15"/>
+      <c r="X19" s="15"/>
       <c r="Y19" s="15"/>
       <c r="Z19" s="15"/>
       <c r="AA19" s="15"/>
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1">
       <c r="A20" s="30" t="s">
-        <v>3773</v>
+        <v>3771</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>3772</v>
-      </c>
-      <c r="E20" s="16"/>
+        <v>65</v>
+      </c>
+      <c r="D20" s="25"/>
+      <c r="E20" s="16" t="s">
+        <v>3795</v>
+      </c>
       <c r="F20" s="29"/>
       <c r="G20" s="29"/>
       <c r="H20" s="29"/>
@@ -14363,58 +14400,58 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1">
       <c r="A21" s="30" t="s">
-        <v>3766</v>
+        <v>3773</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="D21" s="60" t="s">
-        <v>3819</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>3785</v>
-      </c>
-      <c r="F21" s="32"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="16"/>
-      <c r="S21" s="16"/>
-      <c r="T21" s="16"/>
-      <c r="U21" s="16"/>
-      <c r="V21" s="16"/>
-      <c r="W21" s="16"/>
-      <c r="X21" s="16"/>
+      <c r="D21" s="25" t="s">
+        <v>3772</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="29"/>
+      <c r="T21" s="29"/>
+      <c r="U21" s="29"/>
+      <c r="V21" s="29"/>
+      <c r="W21" s="29"/>
+      <c r="X21" s="29"/>
       <c r="Y21" s="15"/>
       <c r="Z21" s="15"/>
       <c r="AA21" s="15"/>
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1">
       <c r="A22" s="30" t="s">
-        <v>3767</v>
+        <v>3766</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>360</v>
-      </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="59" t="s">
-        <v>3801</v>
-      </c>
-      <c r="F22" s="33"/>
+        <v>232</v>
+      </c>
+      <c r="D22" s="60" t="s">
+        <v>3819</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>3785</v>
+      </c>
+      <c r="F22" s="32"/>
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
@@ -14439,51 +14476,55 @@
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1">
       <c r="A23" s="30" t="s">
-        <v>3770</v>
+        <v>3767</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>3752</v>
+        <v>358</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>65</v>
+        <v>360</v>
       </c>
       <c r="D23" s="25"/>
-      <c r="E23" s="16" t="s">
-        <v>3786</v>
-      </c>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="29"/>
-      <c r="N23" s="29"/>
-      <c r="O23" s="29"/>
-      <c r="P23" s="29"/>
-      <c r="Q23" s="29"/>
-      <c r="R23" s="29"/>
-      <c r="S23" s="29"/>
-      <c r="T23" s="29"/>
-      <c r="U23" s="29"/>
-      <c r="V23" s="29"/>
-      <c r="W23" s="29"/>
-      <c r="X23" s="29"/>
+      <c r="E23" s="59" t="s">
+        <v>3801</v>
+      </c>
+      <c r="F23" s="33"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="16"/>
+      <c r="W23" s="16"/>
+      <c r="X23" s="16"/>
       <c r="Y23" s="15"/>
       <c r="Z23" s="15"/>
       <c r="AA23" s="15"/>
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A24" s="30"/>
-      <c r="B24" s="28" t="s">
-        <v>3802</v>
-      </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="60" t="s">
-        <v>3803</v>
-      </c>
-      <c r="E24" s="16"/>
+      <c r="A24" s="30" t="s">
+        <v>3770</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>3752</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="25"/>
+      <c r="E24" s="16" t="s">
+        <v>3786</v>
+      </c>
       <c r="F24" s="29"/>
       <c r="G24" s="29"/>
       <c r="H24" s="29"/>
@@ -14509,14 +14550,16 @@
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1">
       <c r="A25" s="15" t="s">
-        <v>3808</v>
+        <v>3830</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>3809</v>
-      </c>
-      <c r="C25" s="17"/>
+        <v>3828</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>232</v>
+      </c>
       <c r="D25" s="60" t="s">
-        <v>3810</v>
+        <v>3829</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="29"/>
@@ -14543,75 +14586,73 @@
       <c r="AA25" s="15"/>
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A26" s="30" t="s">
-        <v>3768</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>394</v>
+      <c r="A26" s="30"/>
+      <c r="B26" s="28" t="s">
+        <v>3802</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="15" t="s">
-        <v>3787</v>
-      </c>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
-      <c r="T26" s="15"/>
-      <c r="U26" s="15"/>
-      <c r="V26" s="15"/>
-      <c r="W26" s="15"/>
-      <c r="X26" s="15"/>
+      <c r="D26" s="60" t="s">
+        <v>3803</v>
+      </c>
+      <c r="E26" s="16"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="29"/>
+      <c r="Q26" s="29"/>
+      <c r="R26" s="29"/>
+      <c r="S26" s="29"/>
+      <c r="T26" s="29"/>
+      <c r="U26" s="29"/>
+      <c r="V26" s="29"/>
+      <c r="W26" s="29"/>
+      <c r="X26" s="29"/>
       <c r="Y26" s="15"/>
       <c r="Z26" s="15"/>
       <c r="AA26" s="15"/>
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A27" s="30" t="s">
-        <v>3769</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>402</v>
+      <c r="A27" s="15" t="s">
+        <v>3808</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>3809</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="59" t="s">
-        <v>3788</v>
-      </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
-      <c r="T27" s="15"/>
-      <c r="U27" s="15"/>
-      <c r="V27" s="15"/>
-      <c r="W27" s="15"/>
-      <c r="X27" s="15"/>
+      <c r="D27" s="60" t="s">
+        <v>3810</v>
+      </c>
+      <c r="E27" s="16"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="29"/>
+      <c r="R27" s="29"/>
+      <c r="S27" s="29"/>
+      <c r="T27" s="29"/>
+      <c r="U27" s="29"/>
+      <c r="V27" s="29"/>
+      <c r="W27" s="29"/>
+      <c r="X27" s="29"/>
       <c r="Y27" s="15"/>
       <c r="Z27" s="15"/>
       <c r="AA27" s="15"/>
@@ -14621,14 +14662,14 @@
         <v>3768</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>232</v>
       </c>
       <c r="D28" s="25"/>
       <c r="E28" s="15" t="s">
-        <v>3789</v>
+        <v>3787</v>
       </c>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
@@ -14658,14 +14699,14 @@
         <v>3769</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>426</v>
+        <v>402</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>232</v>
       </c>
       <c r="D29" s="25"/>
       <c r="E29" s="59" t="s">
-        <v>3790</v>
+        <v>3788</v>
       </c>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
@@ -14695,13 +14736,15 @@
         <v>3768</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>437</v>
+        <v>412</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>232</v>
       </c>
       <c r="D30" s="25"/>
-      <c r="E30" s="15"/>
+      <c r="E30" s="15" t="s">
+        <v>3789</v>
+      </c>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
@@ -14730,13 +14773,15 @@
         <v>3769</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>467</v>
+        <v>426</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>232</v>
       </c>
       <c r="D31" s="25"/>
-      <c r="E31" s="15"/>
+      <c r="E31" s="59" t="s">
+        <v>3790</v>
+      </c>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
@@ -14761,19 +14806,17 @@
       <c r="AA31" s="15"/>
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A32" s="34" t="s">
-        <v>472</v>
-      </c>
-      <c r="B32" s="28" t="s">
-        <v>477</v>
+      <c r="A32" s="30" t="s">
+        <v>3768</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>437</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="D32" s="25" t="s">
-        <v>3759</v>
-      </c>
-      <c r="E32" s="35"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="15"/>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
@@ -14798,18 +14841,16 @@
       <c r="AA32" s="15"/>
     </row>
     <row r="33" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A33" s="34" t="s">
-        <v>498</v>
-      </c>
-      <c r="B33" s="28" t="s">
-        <v>509</v>
+      <c r="A33" s="30" t="s">
+        <v>3769</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>467</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="D33" s="25" t="s">
-        <v>3759</v>
-      </c>
+      <c r="D33" s="25"/>
       <c r="E33" s="15"/>
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
@@ -14834,12 +14875,12 @@
       <c r="Z33" s="15"/>
       <c r="AA33" s="15"/>
     </row>
-    <row r="34" spans="1:27" ht="16">
+    <row r="34" spans="1:27" ht="15.75" customHeight="1">
       <c r="A34" s="34" t="s">
-        <v>518</v>
+        <v>472</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>519</v>
+        <v>477</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>232</v>
@@ -14847,38 +14888,42 @@
       <c r="D34" s="25" t="s">
         <v>3759</v>
       </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="37"/>
-      <c r="L34" s="37"/>
-      <c r="M34" s="37"/>
-      <c r="N34" s="37"/>
-      <c r="O34" s="37"/>
-      <c r="P34" s="37"/>
-      <c r="Q34" s="37"/>
-      <c r="R34" s="37"/>
-      <c r="S34" s="37"/>
-      <c r="T34" s="37"/>
-      <c r="U34" s="37"/>
-      <c r="V34" s="37"/>
-      <c r="W34" s="37"/>
-      <c r="X34" s="37"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="15"/>
+      <c r="S34" s="15"/>
+      <c r="T34" s="15"/>
+      <c r="U34" s="15"/>
+      <c r="V34" s="15"/>
+      <c r="W34" s="15"/>
+      <c r="X34" s="15"/>
       <c r="Y34" s="15"/>
       <c r="Z34" s="15"/>
       <c r="AA34" s="15"/>
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A35" s="15"/>
-      <c r="B35" s="16" t="s">
-        <v>3823</v>
-      </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="60" t="s">
-        <v>3824</v>
+      <c r="A35" s="34" t="s">
+        <v>498</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>509</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>3759</v>
       </c>
       <c r="E35" s="15"/>
       <c r="F35" s="15"/>
@@ -14904,20 +14949,20 @@
       <c r="Z35" s="15"/>
       <c r="AA35" s="15"/>
     </row>
-    <row r="36" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A36" s="30" t="s">
-        <v>3774</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>3754</v>
+    <row r="36" spans="1:27" ht="16">
+      <c r="A36" s="34" t="s">
+        <v>518</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>519</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="D36" s="25"/>
-      <c r="E36" s="15">
-        <v>1493</v>
-      </c>
+      <c r="D36" s="25" t="s">
+        <v>3759</v>
+      </c>
+      <c r="E36" s="36"/>
       <c r="F36" s="37"/>
       <c r="G36" s="37"/>
       <c r="H36" s="37"/>
@@ -14941,53 +14986,53 @@
       <c r="Z36" s="15"/>
       <c r="AA36" s="15"/>
     </row>
-    <row r="37" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A37" s="30" t="s">
-        <v>3775</v>
-      </c>
+    <row r="37" spans="1:27" ht="48">
+      <c r="A37" s="15"/>
       <c r="B37" s="16" t="s">
-        <v>3755</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="D37" s="25"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="37"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="37"/>
-      <c r="J37" s="37"/>
-      <c r="K37" s="37"/>
-      <c r="L37" s="37"/>
-      <c r="M37" s="37"/>
-      <c r="N37" s="37"/>
-      <c r="O37" s="37"/>
-      <c r="P37" s="37"/>
-      <c r="Q37" s="37"/>
-      <c r="R37" s="37"/>
-      <c r="S37" s="37"/>
-      <c r="T37" s="37"/>
-      <c r="U37" s="37"/>
-      <c r="V37" s="37"/>
-      <c r="W37" s="37"/>
-      <c r="X37" s="37"/>
+        <v>3823</v>
+      </c>
+      <c r="C37" s="17"/>
+      <c r="D37" s="66" t="s">
+        <v>3824</v>
+      </c>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
+      <c r="S37" s="15"/>
+      <c r="T37" s="15"/>
+      <c r="U37" s="15"/>
+      <c r="V37" s="15"/>
+      <c r="W37" s="15"/>
+      <c r="X37" s="15"/>
       <c r="Y37" s="15"/>
       <c r="Z37" s="15"/>
       <c r="AA37" s="15"/>
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
       <c r="A38" s="30" t="s">
-        <v>3776</v>
+        <v>3774</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>3756</v>
+        <v>3754</v>
       </c>
       <c r="C38" s="17" t="s">
         <v>232</v>
       </c>
       <c r="D38" s="25"/>
-      <c r="E38" s="38"/>
+      <c r="E38" s="15">
+        <v>1493</v>
+      </c>
       <c r="F38" s="37"/>
       <c r="G38" s="37"/>
       <c r="H38" s="37"/>
@@ -15013,19 +15058,17 @@
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
       <c r="A39" s="30" t="s">
-        <v>3777</v>
+        <v>3775</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>3757</v>
+        <v>3755</v>
       </c>
       <c r="C39" s="17" t="s">
         <v>232</v>
       </c>
       <c r="D39" s="25"/>
-      <c r="E39" s="15" t="s">
-        <v>3791</v>
-      </c>
-      <c r="F39" s="35"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="37"/>
       <c r="G39" s="37"/>
       <c r="H39" s="37"/>
       <c r="I39" s="37"/>
@@ -15050,89 +15093,89 @@
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
       <c r="A40" s="30" t="s">
-        <v>3778</v>
-      </c>
-      <c r="B40" s="28" t="s">
-        <v>3753</v>
+        <v>3776</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>3756</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>65</v>
+        <v>232</v>
       </c>
       <c r="D40" s="25"/>
-      <c r="E40" s="15" t="s">
-        <v>3792</v>
-      </c>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="15"/>
-      <c r="K40" s="15"/>
-      <c r="L40" s="15"/>
-      <c r="M40" s="15"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="15"/>
-      <c r="P40" s="15"/>
-      <c r="Q40" s="15"/>
-      <c r="R40" s="15"/>
-      <c r="S40" s="15"/>
-      <c r="T40" s="15"/>
-      <c r="U40" s="15"/>
-      <c r="V40" s="15"/>
-      <c r="W40" s="15"/>
-      <c r="X40" s="15"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="37"/>
+      <c r="K40" s="37"/>
+      <c r="L40" s="37"/>
+      <c r="M40" s="37"/>
+      <c r="N40" s="37"/>
+      <c r="O40" s="37"/>
+      <c r="P40" s="37"/>
+      <c r="Q40" s="37"/>
+      <c r="R40" s="37"/>
+      <c r="S40" s="37"/>
+      <c r="T40" s="37"/>
+      <c r="U40" s="37"/>
+      <c r="V40" s="37"/>
+      <c r="W40" s="37"/>
+      <c r="X40" s="37"/>
       <c r="Y40" s="15"/>
       <c r="Z40" s="15"/>
       <c r="AA40" s="15"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A41" s="15" t="s">
-        <v>3804</v>
-      </c>
-      <c r="B41" s="28" t="s">
-        <v>3805</v>
+      <c r="A41" s="30" t="s">
+        <v>3777</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>3757</v>
       </c>
       <c r="C41" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="D41" s="60" t="s">
-        <v>3806</v>
-      </c>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="15"/>
-      <c r="L41" s="15"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="15"/>
-      <c r="O41" s="15"/>
-      <c r="P41" s="15"/>
-      <c r="Q41" s="15"/>
-      <c r="R41" s="15"/>
-      <c r="S41" s="15"/>
-      <c r="T41" s="15"/>
-      <c r="U41" s="15"/>
-      <c r="V41" s="15"/>
-      <c r="W41" s="15"/>
-      <c r="X41" s="15"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="15" t="s">
+        <v>3791</v>
+      </c>
+      <c r="F41" s="35"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="37"/>
+      <c r="L41" s="37"/>
+      <c r="M41" s="37"/>
+      <c r="N41" s="37"/>
+      <c r="O41" s="37"/>
+      <c r="P41" s="37"/>
+      <c r="Q41" s="37"/>
+      <c r="R41" s="37"/>
+      <c r="S41" s="37"/>
+      <c r="T41" s="37"/>
+      <c r="U41" s="37"/>
+      <c r="V41" s="37"/>
+      <c r="W41" s="37"/>
+      <c r="X41" s="37"/>
       <c r="Y41" s="15"/>
       <c r="Z41" s="15"/>
       <c r="AA41" s="15"/>
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1">
       <c r="A42" s="30" t="s">
-        <v>3779</v>
-      </c>
-      <c r="B42" s="39" t="s">
-        <v>3760</v>
-      </c>
-      <c r="C42" s="17"/>
+        <v>3778</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>3753</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>65</v>
+      </c>
       <c r="D42" s="25"/>
       <c r="E42" s="15" t="s">
-        <v>3793</v>
+        <v>3792</v>
       </c>
       <c r="F42" s="15"/>
       <c r="G42" s="15"/>
@@ -15159,18 +15202,18 @@
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1">
       <c r="A43" s="15" t="s">
-        <v>3820</v>
+        <v>3804</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>3821</v>
-      </c>
-      <c r="C43" s="17"/>
+        <v>3805</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>232</v>
+      </c>
       <c r="D43" s="60" t="s">
         <v>3806</v>
       </c>
-      <c r="E43" s="15" t="s">
-        <v>3822</v>
-      </c>
+      <c r="E43" s="15"/>
       <c r="F43" s="15"/>
       <c r="G43" s="15"/>
       <c r="H43" s="15"/>
@@ -15194,47 +15237,55 @@
       <c r="Z43" s="15"/>
       <c r="AA43" s="15"/>
     </row>
-    <row r="44" spans="1:27" s="45" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A44" s="34" t="s">
-        <v>638</v>
-      </c>
-      <c r="B44" s="40" t="s">
-        <v>639</v>
-      </c>
-      <c r="C44" s="42" t="s">
-        <v>232</v>
-      </c>
-      <c r="D44" s="43"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="46"/>
-      <c r="G44" s="46"/>
-      <c r="H44" s="46"/>
-      <c r="I44" s="46"/>
-      <c r="J44" s="46"/>
-      <c r="K44" s="46"/>
-      <c r="L44" s="46"/>
-      <c r="M44" s="46"/>
-      <c r="N44" s="46"/>
-      <c r="O44" s="46"/>
-      <c r="P44" s="46"/>
-      <c r="Q44" s="46"/>
-      <c r="R44" s="46"/>
-      <c r="S44" s="46"/>
-      <c r="T44" s="46"/>
-      <c r="U44" s="46"/>
-      <c r="V44" s="46"/>
-      <c r="W44" s="46"/>
-      <c r="X44" s="46"/>
-      <c r="Y44" s="34"/>
-      <c r="Z44" s="34"/>
-      <c r="AA44" s="34"/>
+    <row r="44" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A44" s="30" t="s">
+        <v>3779</v>
+      </c>
+      <c r="B44" s="39" t="s">
+        <v>3760</v>
+      </c>
+      <c r="C44" s="17"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="15" t="s">
+        <v>3793</v>
+      </c>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="15"/>
+      <c r="S44" s="15"/>
+      <c r="T44" s="15"/>
+      <c r="U44" s="15"/>
+      <c r="V44" s="15"/>
+      <c r="W44" s="15"/>
+      <c r="X44" s="15"/>
+      <c r="Y44" s="15"/>
+      <c r="Z44" s="15"/>
+      <c r="AA44" s="15"/>
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A45" s="15"/>
-      <c r="B45" s="16"/>
+      <c r="A45" s="15" t="s">
+        <v>3820</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>3821</v>
+      </c>
       <c r="C45" s="17"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="15"/>
+      <c r="D45" s="60" t="s">
+        <v>3806</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>3822</v>
+      </c>
       <c r="F45" s="15"/>
       <c r="G45" s="15"/>
       <c r="H45" s="15"/>
@@ -15260,16 +15311,16 @@
     </row>
     <row r="46" spans="1:27" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A46" s="34" t="s">
-        <v>647</v>
+        <v>638</v>
       </c>
       <c r="B46" s="40" t="s">
-        <v>648</v>
+        <v>639</v>
       </c>
       <c r="C46" s="42" t="s">
         <v>232</v>
       </c>
       <c r="D46" s="43"/>
-      <c r="E46" s="57"/>
+      <c r="E46" s="34"/>
       <c r="F46" s="46"/>
       <c r="G46" s="46"/>
       <c r="H46" s="46"/>
@@ -15294,19 +15345,11 @@
       <c r="AA46" s="34"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A47" s="30" t="s">
-        <v>3780</v>
-      </c>
-      <c r="B47" s="16" t="s">
-        <v>665</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>65</v>
-      </c>
+      <c r="A47" s="15"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="17"/>
       <c r="D47" s="25"/>
-      <c r="E47" s="15" t="s">
-        <v>666</v>
-      </c>
+      <c r="E47" s="15"/>
       <c r="F47" s="15"/>
       <c r="G47" s="15"/>
       <c r="H47" s="15"/>
@@ -15330,164 +15373,166 @@
       <c r="Z47" s="15"/>
       <c r="AA47" s="15"/>
     </row>
-    <row r="48" spans="1:27" ht="16">
-      <c r="A48" s="30" t="s">
-        <v>3781</v>
-      </c>
-      <c r="B48" s="41" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C48" s="17" t="s">
+    <row r="48" spans="1:27" s="45" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A48" s="34" t="s">
+        <v>647</v>
+      </c>
+      <c r="B48" s="40" t="s">
+        <v>648</v>
+      </c>
+      <c r="C48" s="42" t="s">
         <v>232</v>
       </c>
-      <c r="D48" s="25" t="s">
-        <v>3764</v>
-      </c>
-      <c r="E48" s="36" t="s">
-        <v>3794</v>
-      </c>
-      <c r="F48" s="37"/>
-      <c r="G48" s="37"/>
-      <c r="H48" s="37"/>
-      <c r="I48" s="37"/>
-      <c r="J48" s="37"/>
-      <c r="K48" s="37"/>
-      <c r="L48" s="37"/>
-      <c r="M48" s="37"/>
-      <c r="N48" s="37"/>
-      <c r="O48" s="37"/>
-      <c r="P48" s="37"/>
-      <c r="Q48" s="37"/>
-      <c r="R48" s="37"/>
-      <c r="S48" s="37"/>
-      <c r="T48" s="37"/>
-      <c r="U48" s="37"/>
-      <c r="V48" s="37"/>
-      <c r="W48" s="37"/>
-      <c r="X48" s="37"/>
-      <c r="Y48" s="15"/>
-      <c r="Z48" s="15"/>
-      <c r="AA48" s="15"/>
-    </row>
-    <row r="49" spans="1:27" ht="16">
+      <c r="D48" s="43"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="46"/>
+      <c r="I48" s="46"/>
+      <c r="J48" s="46"/>
+      <c r="K48" s="46"/>
+      <c r="L48" s="46"/>
+      <c r="M48" s="46"/>
+      <c r="N48" s="46"/>
+      <c r="O48" s="46"/>
+      <c r="P48" s="46"/>
+      <c r="Q48" s="46"/>
+      <c r="R48" s="46"/>
+      <c r="S48" s="46"/>
+      <c r="T48" s="46"/>
+      <c r="U48" s="46"/>
+      <c r="V48" s="46"/>
+      <c r="W48" s="46"/>
+      <c r="X48" s="46"/>
+      <c r="Y48" s="34"/>
+      <c r="Z48" s="34"/>
+      <c r="AA48" s="34"/>
+    </row>
+    <row r="49" spans="1:27" ht="15.75" customHeight="1">
       <c r="A49" s="30" t="s">
-        <v>3781</v>
-      </c>
-      <c r="B49" s="41" t="s">
-        <v>3762</v>
-      </c>
-      <c r="C49" s="17"/>
-      <c r="D49" s="25" t="s">
-        <v>3763</v>
-      </c>
-      <c r="E49" s="36" t="s">
-        <v>3796</v>
-      </c>
-      <c r="F49" s="37"/>
-      <c r="G49" s="37"/>
-      <c r="H49" s="37"/>
-      <c r="I49" s="37"/>
-      <c r="J49" s="37"/>
-      <c r="K49" s="37"/>
-      <c r="L49" s="37"/>
-      <c r="M49" s="37"/>
-      <c r="N49" s="37"/>
-      <c r="O49" s="37"/>
-      <c r="P49" s="37"/>
-      <c r="Q49" s="37"/>
-      <c r="R49" s="37"/>
-      <c r="S49" s="37"/>
-      <c r="T49" s="37"/>
-      <c r="U49" s="37"/>
-      <c r="V49" s="37"/>
-      <c r="W49" s="37"/>
-      <c r="X49" s="37"/>
+        <v>3780</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>665</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49" s="25"/>
+      <c r="E49" s="15" t="s">
+        <v>666</v>
+      </c>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="15"/>
+      <c r="K49" s="15"/>
+      <c r="L49" s="15"/>
+      <c r="M49" s="15"/>
+      <c r="N49" s="15"/>
+      <c r="O49" s="15"/>
+      <c r="P49" s="15"/>
+      <c r="Q49" s="15"/>
+      <c r="R49" s="15"/>
+      <c r="S49" s="15"/>
+      <c r="T49" s="15"/>
+      <c r="U49" s="15"/>
+      <c r="V49" s="15"/>
+      <c r="W49" s="15"/>
+      <c r="X49" s="15"/>
       <c r="Y49" s="15"/>
       <c r="Z49" s="15"/>
       <c r="AA49" s="15"/>
     </row>
-    <row r="50" spans="1:27" s="45" customFormat="1" ht="16">
-      <c r="A50" s="34" t="s">
-        <v>676</v>
-      </c>
-      <c r="B50" s="40" t="s">
-        <v>678</v>
-      </c>
-      <c r="C50" s="42" t="s">
+    <row r="50" spans="1:27" ht="16">
+      <c r="A50" s="30" t="s">
+        <v>3781</v>
+      </c>
+      <c r="B50" s="41" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C50" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="D50" s="43"/>
-      <c r="E50" s="44"/>
-      <c r="F50" s="46"/>
-      <c r="G50" s="46"/>
-      <c r="H50" s="46"/>
-      <c r="I50" s="46"/>
-      <c r="J50" s="46"/>
-      <c r="K50" s="46"/>
-      <c r="L50" s="46"/>
-      <c r="M50" s="46"/>
-      <c r="N50" s="46"/>
-      <c r="O50" s="46"/>
-      <c r="P50" s="46"/>
-      <c r="Q50" s="46"/>
-      <c r="R50" s="46"/>
-      <c r="S50" s="46"/>
-      <c r="T50" s="46"/>
-      <c r="U50" s="46"/>
-      <c r="V50" s="46"/>
-      <c r="W50" s="46"/>
-      <c r="X50" s="46"/>
-      <c r="Y50" s="34"/>
-      <c r="Z50" s="34"/>
-      <c r="AA50" s="34"/>
-    </row>
-    <row r="51" spans="1:27" s="45" customFormat="1" ht="16">
-      <c r="A51" s="34" t="s">
-        <v>684</v>
-      </c>
-      <c r="B51" s="40" t="s">
-        <v>686</v>
-      </c>
-      <c r="C51" s="42" t="s">
-        <v>232</v>
-      </c>
-      <c r="D51" s="43"/>
-      <c r="E51" s="44"/>
-      <c r="F51" s="34"/>
-      <c r="G51" s="34"/>
-      <c r="H51" s="34"/>
-      <c r="I51" s="34"/>
-      <c r="J51" s="34"/>
-      <c r="K51" s="34"/>
-      <c r="L51" s="34"/>
-      <c r="M51" s="34"/>
-      <c r="N51" s="34"/>
-      <c r="O51" s="34"/>
-      <c r="P51" s="34"/>
-      <c r="Q51" s="34"/>
-      <c r="R51" s="34"/>
-      <c r="S51" s="34"/>
-      <c r="T51" s="34"/>
-      <c r="U51" s="34"/>
-      <c r="V51" s="34"/>
-      <c r="W51" s="34"/>
-      <c r="X51" s="34"/>
-      <c r="Y51" s="34"/>
-      <c r="Z51" s="34"/>
-      <c r="AA51" s="34"/>
+      <c r="D50" s="25" t="s">
+        <v>3764</v>
+      </c>
+      <c r="E50" s="36" t="s">
+        <v>3794</v>
+      </c>
+      <c r="F50" s="37"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="37"/>
+      <c r="J50" s="37"/>
+      <c r="K50" s="37"/>
+      <c r="L50" s="37"/>
+      <c r="M50" s="37"/>
+      <c r="N50" s="37"/>
+      <c r="O50" s="37"/>
+      <c r="P50" s="37"/>
+      <c r="Q50" s="37"/>
+      <c r="R50" s="37"/>
+      <c r="S50" s="37"/>
+      <c r="T50" s="37"/>
+      <c r="U50" s="37"/>
+      <c r="V50" s="37"/>
+      <c r="W50" s="37"/>
+      <c r="X50" s="37"/>
+      <c r="Y50" s="15"/>
+      <c r="Z50" s="15"/>
+      <c r="AA50" s="15"/>
+    </row>
+    <row r="51" spans="1:27" ht="16">
+      <c r="A51" s="30" t="s">
+        <v>3781</v>
+      </c>
+      <c r="B51" s="41" t="s">
+        <v>3762</v>
+      </c>
+      <c r="C51" s="17"/>
+      <c r="D51" s="25" t="s">
+        <v>3763</v>
+      </c>
+      <c r="E51" s="36" t="s">
+        <v>3796</v>
+      </c>
+      <c r="F51" s="37"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="37"/>
+      <c r="J51" s="37"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="37"/>
+      <c r="M51" s="37"/>
+      <c r="N51" s="37"/>
+      <c r="O51" s="37"/>
+      <c r="P51" s="37"/>
+      <c r="Q51" s="37"/>
+      <c r="R51" s="37"/>
+      <c r="S51" s="37"/>
+      <c r="T51" s="37"/>
+      <c r="U51" s="37"/>
+      <c r="V51" s="37"/>
+      <c r="W51" s="37"/>
+      <c r="X51" s="37"/>
+      <c r="Y51" s="15"/>
+      <c r="Z51" s="15"/>
+      <c r="AA51" s="15"/>
     </row>
     <row r="52" spans="1:27" s="45" customFormat="1" ht="16">
       <c r="A52" s="34" t="s">
-        <v>691</v>
+        <v>676</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>693</v>
+        <v>678</v>
       </c>
       <c r="C52" s="42" t="s">
         <v>232</v>
       </c>
       <c r="D52" s="43"/>
-      <c r="E52" s="34"/>
+      <c r="E52" s="44"/>
       <c r="F52" s="46"/>
       <c r="G52" s="46"/>
       <c r="H52" s="46"/>
@@ -15513,86 +15558,86 @@
     </row>
     <row r="53" spans="1:27" s="45" customFormat="1" ht="16">
       <c r="A53" s="34" t="s">
-        <v>699</v>
+        <v>684</v>
       </c>
       <c r="B53" s="40" t="s">
-        <v>700</v>
+        <v>686</v>
       </c>
       <c r="C53" s="42" t="s">
         <v>232</v>
       </c>
       <c r="D53" s="43"/>
-      <c r="E53" s="47"/>
-      <c r="F53" s="46"/>
-      <c r="G53" s="46"/>
-      <c r="H53" s="46"/>
-      <c r="I53" s="46"/>
-      <c r="J53" s="46"/>
-      <c r="K53" s="46"/>
-      <c r="L53" s="46"/>
-      <c r="M53" s="46"/>
-      <c r="N53" s="46"/>
-      <c r="O53" s="46"/>
-      <c r="P53" s="46"/>
-      <c r="Q53" s="46"/>
-      <c r="R53" s="46"/>
-      <c r="S53" s="46"/>
-      <c r="T53" s="46"/>
-      <c r="U53" s="46"/>
-      <c r="V53" s="46"/>
-      <c r="W53" s="46"/>
-      <c r="X53" s="46"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="34"/>
+      <c r="G53" s="34"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="34"/>
+      <c r="J53" s="34"/>
+      <c r="K53" s="34"/>
+      <c r="L53" s="34"/>
+      <c r="M53" s="34"/>
+      <c r="N53" s="34"/>
+      <c r="O53" s="34"/>
+      <c r="P53" s="34"/>
+      <c r="Q53" s="34"/>
+      <c r="R53" s="34"/>
+      <c r="S53" s="34"/>
+      <c r="T53" s="34"/>
+      <c r="U53" s="34"/>
+      <c r="V53" s="34"/>
+      <c r="W53" s="34"/>
+      <c r="X53" s="34"/>
       <c r="Y53" s="34"/>
       <c r="Z53" s="34"/>
       <c r="AA53" s="34"/>
     </row>
     <row r="54" spans="1:27" s="45" customFormat="1" ht="16">
       <c r="A54" s="34" t="s">
-        <v>714</v>
+        <v>691</v>
       </c>
       <c r="B54" s="40" t="s">
-        <v>718</v>
+        <v>693</v>
       </c>
       <c r="C54" s="42" t="s">
         <v>232</v>
       </c>
       <c r="D54" s="43"/>
       <c r="E54" s="34"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="34"/>
-      <c r="H54" s="34"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="34"/>
-      <c r="K54" s="34"/>
-      <c r="L54" s="34"/>
-      <c r="M54" s="34"/>
-      <c r="N54" s="34"/>
-      <c r="O54" s="34"/>
-      <c r="P54" s="34"/>
-      <c r="Q54" s="34"/>
-      <c r="R54" s="34"/>
-      <c r="S54" s="34"/>
-      <c r="T54" s="34"/>
-      <c r="U54" s="34"/>
-      <c r="V54" s="34"/>
-      <c r="W54" s="34"/>
-      <c r="X54" s="34"/>
+      <c r="F54" s="46"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="46"/>
+      <c r="I54" s="46"/>
+      <c r="J54" s="46"/>
+      <c r="K54" s="46"/>
+      <c r="L54" s="46"/>
+      <c r="M54" s="46"/>
+      <c r="N54" s="46"/>
+      <c r="O54" s="46"/>
+      <c r="P54" s="46"/>
+      <c r="Q54" s="46"/>
+      <c r="R54" s="46"/>
+      <c r="S54" s="46"/>
+      <c r="T54" s="46"/>
+      <c r="U54" s="46"/>
+      <c r="V54" s="46"/>
+      <c r="W54" s="46"/>
+      <c r="X54" s="46"/>
       <c r="Y54" s="34"/>
       <c r="Z54" s="34"/>
       <c r="AA54" s="34"/>
     </row>
     <row r="55" spans="1:27" s="45" customFormat="1" ht="16">
       <c r="A55" s="34" t="s">
-        <v>729</v>
+        <v>699</v>
       </c>
       <c r="B55" s="40" t="s">
-        <v>733</v>
+        <v>700</v>
       </c>
       <c r="C55" s="42" t="s">
         <v>232</v>
       </c>
       <c r="D55" s="43"/>
-      <c r="E55" s="44"/>
+      <c r="E55" s="47"/>
       <c r="F55" s="46"/>
       <c r="G55" s="46"/>
       <c r="H55" s="46"/>
@@ -15618,86 +15663,86 @@
     </row>
     <row r="56" spans="1:27" s="45" customFormat="1" ht="16">
       <c r="A56" s="34" t="s">
-        <v>743</v>
+        <v>714</v>
       </c>
       <c r="B56" s="40" t="s">
-        <v>744</v>
+        <v>718</v>
       </c>
       <c r="C56" s="42" t="s">
         <v>232</v>
       </c>
       <c r="D56" s="43"/>
-      <c r="E56" s="44"/>
-      <c r="F56" s="46"/>
-      <c r="G56" s="46"/>
-      <c r="H56" s="46"/>
-      <c r="I56" s="46"/>
-      <c r="J56" s="46"/>
-      <c r="K56" s="46"/>
-      <c r="L56" s="46"/>
-      <c r="M56" s="46"/>
-      <c r="N56" s="46"/>
-      <c r="O56" s="46"/>
-      <c r="P56" s="46"/>
-      <c r="Q56" s="46"/>
-      <c r="R56" s="46"/>
-      <c r="S56" s="46"/>
-      <c r="T56" s="46"/>
-      <c r="U56" s="46"/>
-      <c r="V56" s="46"/>
-      <c r="W56" s="46"/>
-      <c r="X56" s="46"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="34"/>
+      <c r="G56" s="34"/>
+      <c r="H56" s="34"/>
+      <c r="I56" s="34"/>
+      <c r="J56" s="34"/>
+      <c r="K56" s="34"/>
+      <c r="L56" s="34"/>
+      <c r="M56" s="34"/>
+      <c r="N56" s="34"/>
+      <c r="O56" s="34"/>
+      <c r="P56" s="34"/>
+      <c r="Q56" s="34"/>
+      <c r="R56" s="34"/>
+      <c r="S56" s="34"/>
+      <c r="T56" s="34"/>
+      <c r="U56" s="34"/>
+      <c r="V56" s="34"/>
+      <c r="W56" s="34"/>
+      <c r="X56" s="34"/>
       <c r="Y56" s="34"/>
       <c r="Z56" s="34"/>
       <c r="AA56" s="34"/>
     </row>
     <row r="57" spans="1:27" s="45" customFormat="1" ht="16">
       <c r="A57" s="34" t="s">
-        <v>747</v>
+        <v>729</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>748</v>
+        <v>733</v>
       </c>
       <c r="C57" s="42" t="s">
         <v>232</v>
       </c>
       <c r="D57" s="43"/>
       <c r="E57" s="44"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="48"/>
-      <c r="I57" s="48"/>
-      <c r="J57" s="48"/>
-      <c r="K57" s="48"/>
-      <c r="L57" s="48"/>
-      <c r="M57" s="48"/>
-      <c r="N57" s="48"/>
-      <c r="O57" s="48"/>
-      <c r="P57" s="48"/>
-      <c r="Q57" s="48"/>
-      <c r="R57" s="48"/>
-      <c r="S57" s="48"/>
-      <c r="T57" s="48"/>
-      <c r="U57" s="48"/>
-      <c r="V57" s="48"/>
-      <c r="W57" s="48"/>
-      <c r="X57" s="48"/>
-      <c r="Y57" s="49"/>
-      <c r="Z57" s="50"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="46"/>
+      <c r="I57" s="46"/>
+      <c r="J57" s="46"/>
+      <c r="K57" s="46"/>
+      <c r="L57" s="46"/>
+      <c r="M57" s="46"/>
+      <c r="N57" s="46"/>
+      <c r="O57" s="46"/>
+      <c r="P57" s="46"/>
+      <c r="Q57" s="46"/>
+      <c r="R57" s="46"/>
+      <c r="S57" s="46"/>
+      <c r="T57" s="46"/>
+      <c r="U57" s="46"/>
+      <c r="V57" s="46"/>
+      <c r="W57" s="46"/>
+      <c r="X57" s="46"/>
+      <c r="Y57" s="34"/>
+      <c r="Z57" s="34"/>
       <c r="AA57" s="34"/>
     </row>
     <row r="58" spans="1:27" s="45" customFormat="1" ht="16">
       <c r="A58" s="34" t="s">
-        <v>784</v>
+        <v>743</v>
       </c>
       <c r="B58" s="40" t="s">
-        <v>786</v>
+        <v>744</v>
       </c>
       <c r="C58" s="42" t="s">
         <v>232</v>
       </c>
       <c r="D58" s="43"/>
-      <c r="E58" s="34"/>
+      <c r="E58" s="44"/>
       <c r="F58" s="46"/>
       <c r="G58" s="46"/>
       <c r="H58" s="46"/>
@@ -15717,188 +15762,188 @@
       <c r="V58" s="46"/>
       <c r="W58" s="46"/>
       <c r="X58" s="46"/>
-      <c r="Y58" s="49"/>
-      <c r="Z58" s="50"/>
+      <c r="Y58" s="34"/>
+      <c r="Z58" s="34"/>
       <c r="AA58" s="34"/>
     </row>
     <row r="59" spans="1:27" s="45" customFormat="1" ht="16">
       <c r="A59" s="34" t="s">
-        <v>792</v>
+        <v>747</v>
       </c>
       <c r="B59" s="40" t="s">
-        <v>794</v>
+        <v>748</v>
       </c>
       <c r="C59" s="42" t="s">
         <v>232</v>
       </c>
       <c r="D59" s="43"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="46"/>
-      <c r="G59" s="46"/>
-      <c r="H59" s="46"/>
-      <c r="I59" s="46"/>
-      <c r="J59" s="46"/>
-      <c r="K59" s="46"/>
-      <c r="L59" s="46"/>
-      <c r="M59" s="46"/>
-      <c r="N59" s="46"/>
-      <c r="O59" s="46"/>
-      <c r="P59" s="46"/>
-      <c r="Q59" s="46"/>
-      <c r="R59" s="46"/>
-      <c r="S59" s="46"/>
-      <c r="T59" s="46"/>
-      <c r="U59" s="46"/>
-      <c r="V59" s="46"/>
-      <c r="W59" s="46"/>
-      <c r="X59" s="46"/>
-      <c r="Y59" s="34"/>
-      <c r="Z59" s="34"/>
+      <c r="E59" s="44"/>
+      <c r="F59" s="48"/>
+      <c r="G59" s="48"/>
+      <c r="H59" s="48"/>
+      <c r="I59" s="48"/>
+      <c r="J59" s="48"/>
+      <c r="K59" s="48"/>
+      <c r="L59" s="48"/>
+      <c r="M59" s="48"/>
+      <c r="N59" s="48"/>
+      <c r="O59" s="48"/>
+      <c r="P59" s="48"/>
+      <c r="Q59" s="48"/>
+      <c r="R59" s="48"/>
+      <c r="S59" s="48"/>
+      <c r="T59" s="48"/>
+      <c r="U59" s="48"/>
+      <c r="V59" s="48"/>
+      <c r="W59" s="48"/>
+      <c r="X59" s="48"/>
+      <c r="Y59" s="49"/>
+      <c r="Z59" s="50"/>
       <c r="AA59" s="34"/>
     </row>
-    <row r="60" spans="1:27" ht="16">
-      <c r="A60" s="30" t="s">
+    <row r="60" spans="1:27" s="45" customFormat="1" ht="16">
+      <c r="A60" s="34" t="s">
+        <v>784</v>
+      </c>
+      <c r="B60" s="40" t="s">
+        <v>786</v>
+      </c>
+      <c r="C60" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="D60" s="43"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="46"/>
+      <c r="G60" s="46"/>
+      <c r="H60" s="46"/>
+      <c r="I60" s="46"/>
+      <c r="J60" s="46"/>
+      <c r="K60" s="46"/>
+      <c r="L60" s="46"/>
+      <c r="M60" s="46"/>
+      <c r="N60" s="46"/>
+      <c r="O60" s="46"/>
+      <c r="P60" s="46"/>
+      <c r="Q60" s="46"/>
+      <c r="R60" s="46"/>
+      <c r="S60" s="46"/>
+      <c r="T60" s="46"/>
+      <c r="U60" s="46"/>
+      <c r="V60" s="46"/>
+      <c r="W60" s="46"/>
+      <c r="X60" s="46"/>
+      <c r="Y60" s="49"/>
+      <c r="Z60" s="50"/>
+      <c r="AA60" s="34"/>
+    </row>
+    <row r="61" spans="1:27" s="45" customFormat="1" ht="16">
+      <c r="A61" s="34" t="s">
+        <v>792</v>
+      </c>
+      <c r="B61" s="40" t="s">
+        <v>794</v>
+      </c>
+      <c r="C61" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="D61" s="43"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="46"/>
+      <c r="G61" s="46"/>
+      <c r="H61" s="46"/>
+      <c r="I61" s="46"/>
+      <c r="J61" s="46"/>
+      <c r="K61" s="46"/>
+      <c r="L61" s="46"/>
+      <c r="M61" s="46"/>
+      <c r="N61" s="46"/>
+      <c r="O61" s="46"/>
+      <c r="P61" s="46"/>
+      <c r="Q61" s="46"/>
+      <c r="R61" s="46"/>
+      <c r="S61" s="46"/>
+      <c r="T61" s="46"/>
+      <c r="U61" s="46"/>
+      <c r="V61" s="46"/>
+      <c r="W61" s="46"/>
+      <c r="X61" s="46"/>
+      <c r="Y61" s="34"/>
+      <c r="Z61" s="34"/>
+      <c r="AA61" s="34"/>
+    </row>
+    <row r="62" spans="1:27" ht="16">
+      <c r="A62" s="30" t="s">
         <v>3782</v>
       </c>
-      <c r="B60" s="16" t="s">
+      <c r="B62" s="16" t="s">
         <v>802</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C62" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="D60" s="25"/>
-      <c r="E60" s="15"/>
-      <c r="F60" s="15"/>
-      <c r="G60" s="15"/>
-      <c r="H60" s="15"/>
-      <c r="I60" s="15"/>
-      <c r="J60" s="15"/>
-      <c r="K60" s="15"/>
-      <c r="L60" s="15"/>
-      <c r="M60" s="15"/>
-      <c r="N60" s="15"/>
-      <c r="O60" s="15"/>
-      <c r="P60" s="15"/>
-      <c r="Q60" s="15"/>
-      <c r="R60" s="15"/>
-      <c r="S60" s="15"/>
-      <c r="T60" s="15"/>
-      <c r="U60" s="15"/>
-      <c r="V60" s="15"/>
-      <c r="W60" s="15"/>
-      <c r="X60" s="15"/>
-      <c r="Y60" s="15"/>
-      <c r="Z60" s="15"/>
-      <c r="AA60" s="15"/>
-    </row>
-    <row r="61" spans="1:27" ht="16">
-      <c r="A61" s="15"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="15"/>
-      <c r="F61" s="15"/>
-      <c r="G61" s="15"/>
-      <c r="H61" s="15"/>
-      <c r="I61" s="15"/>
-      <c r="J61" s="15"/>
-      <c r="K61" s="15"/>
-      <c r="L61" s="15"/>
-      <c r="M61" s="15"/>
-      <c r="N61" s="15"/>
-      <c r="O61" s="15"/>
-      <c r="P61" s="15"/>
-      <c r="Q61" s="15"/>
-      <c r="R61" s="15"/>
-      <c r="S61" s="15"/>
-      <c r="T61" s="15"/>
-      <c r="U61" s="15"/>
-      <c r="V61" s="15"/>
-      <c r="W61" s="15"/>
-      <c r="X61" s="15"/>
-      <c r="Y61" s="15"/>
-      <c r="Z61" s="15"/>
-      <c r="AA61" s="15"/>
-    </row>
-    <row r="62" spans="1:27" s="45" customFormat="1" ht="16">
-      <c r="A62" s="34" t="s">
-        <v>814</v>
-      </c>
-      <c r="B62" s="40" t="s">
-        <v>816</v>
-      </c>
-      <c r="C62" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="D62" s="43"/>
-      <c r="E62" s="34"/>
-      <c r="F62" s="46"/>
-      <c r="G62" s="46"/>
-      <c r="H62" s="46"/>
-      <c r="I62" s="46"/>
-      <c r="J62" s="46"/>
-      <c r="K62" s="46"/>
-      <c r="L62" s="46"/>
-      <c r="M62" s="46"/>
-      <c r="N62" s="46"/>
-      <c r="O62" s="46"/>
-      <c r="P62" s="46"/>
-      <c r="Q62" s="46"/>
-      <c r="R62" s="46"/>
-      <c r="S62" s="46"/>
-      <c r="T62" s="46"/>
-      <c r="U62" s="46"/>
-      <c r="V62" s="46"/>
-      <c r="W62" s="46"/>
-      <c r="X62" s="46"/>
-      <c r="Y62" s="34"/>
-      <c r="Z62" s="34"/>
-      <c r="AA62" s="34"/>
-    </row>
-    <row r="63" spans="1:27" s="45" customFormat="1" ht="16">
-      <c r="A63" s="34" t="s">
-        <v>676</v>
-      </c>
-      <c r="B63" s="40" t="s">
-        <v>827</v>
-      </c>
-      <c r="C63" s="42" t="s">
-        <v>232</v>
-      </c>
-      <c r="D63" s="43"/>
-      <c r="E63" s="34"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="34"/>
-      <c r="H63" s="34"/>
-      <c r="I63" s="34"/>
-      <c r="J63" s="34"/>
-      <c r="K63" s="34"/>
-      <c r="L63" s="34"/>
-      <c r="M63" s="34"/>
-      <c r="N63" s="34"/>
-      <c r="O63" s="34"/>
-      <c r="P63" s="34"/>
-      <c r="Q63" s="34"/>
-      <c r="R63" s="34"/>
-      <c r="S63" s="34"/>
-      <c r="T63" s="34"/>
-      <c r="U63" s="34"/>
-      <c r="V63" s="34"/>
-      <c r="W63" s="34"/>
-      <c r="X63" s="34"/>
-      <c r="Y63" s="34"/>
-      <c r="Z63" s="34"/>
-      <c r="AA63" s="34"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+      <c r="J62" s="15"/>
+      <c r="K62" s="15"/>
+      <c r="L62" s="15"/>
+      <c r="M62" s="15"/>
+      <c r="N62" s="15"/>
+      <c r="O62" s="15"/>
+      <c r="P62" s="15"/>
+      <c r="Q62" s="15"/>
+      <c r="R62" s="15"/>
+      <c r="S62" s="15"/>
+      <c r="T62" s="15"/>
+      <c r="U62" s="15"/>
+      <c r="V62" s="15"/>
+      <c r="W62" s="15"/>
+      <c r="X62" s="15"/>
+      <c r="Y62" s="15"/>
+      <c r="Z62" s="15"/>
+      <c r="AA62" s="15"/>
+    </row>
+    <row r="63" spans="1:27" ht="16">
+      <c r="A63" s="15"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="15"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="15"/>
+      <c r="M63" s="15"/>
+      <c r="N63" s="15"/>
+      <c r="O63" s="15"/>
+      <c r="P63" s="15"/>
+      <c r="Q63" s="15"/>
+      <c r="R63" s="15"/>
+      <c r="S63" s="15"/>
+      <c r="T63" s="15"/>
+      <c r="U63" s="15"/>
+      <c r="V63" s="15"/>
+      <c r="W63" s="15"/>
+      <c r="X63" s="15"/>
+      <c r="Y63" s="15"/>
+      <c r="Z63" s="15"/>
+      <c r="AA63" s="15"/>
     </row>
     <row r="64" spans="1:27" s="45" customFormat="1" ht="16">
       <c r="A64" s="34" t="s">
-        <v>676</v>
+        <v>814</v>
       </c>
       <c r="B64" s="40" t="s">
-        <v>837</v>
+        <v>816</v>
       </c>
       <c r="C64" s="42" t="s">
-        <v>232</v>
+        <v>65</v>
       </c>
       <c r="D64" s="43"/>
       <c r="E64" s="34"/>
@@ -15925,82 +15970,82 @@
       <c r="Z64" s="34"/>
       <c r="AA64" s="34"/>
     </row>
-    <row r="65" spans="1:27" ht="16">
-      <c r="A65" s="15"/>
-      <c r="B65" s="16"/>
-      <c r="C65" s="17"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="15"/>
-      <c r="F65" s="15"/>
-      <c r="G65" s="15"/>
-      <c r="H65" s="15"/>
-      <c r="I65" s="15"/>
-      <c r="J65" s="15"/>
-      <c r="K65" s="15"/>
-      <c r="L65" s="15"/>
-      <c r="M65" s="15"/>
-      <c r="N65" s="15"/>
-      <c r="O65" s="15"/>
-      <c r="P65" s="15"/>
-      <c r="Q65" s="15"/>
-      <c r="R65" s="15"/>
-      <c r="S65" s="15"/>
-      <c r="T65" s="15"/>
-      <c r="U65" s="15"/>
-      <c r="V65" s="15"/>
-      <c r="W65" s="15"/>
-      <c r="X65" s="15"/>
-      <c r="Y65" s="15"/>
-      <c r="Z65" s="15"/>
-      <c r="AA65" s="15"/>
-    </row>
-    <row r="66" spans="1:27" ht="16">
-      <c r="A66" s="58" t="s">
-        <v>3783</v>
-      </c>
-      <c r="B66" s="51" t="s">
-        <v>869</v>
-      </c>
-      <c r="C66" s="52" t="s">
+    <row r="65" spans="1:27" s="45" customFormat="1" ht="16">
+      <c r="A65" s="34" t="s">
+        <v>676</v>
+      </c>
+      <c r="B65" s="40" t="s">
+        <v>827</v>
+      </c>
+      <c r="C65" s="42" t="s">
         <v>232</v>
       </c>
-      <c r="D66" s="53"/>
-      <c r="E66" s="15"/>
-      <c r="F66" s="54"/>
-      <c r="G66" s="15"/>
-      <c r="H66" s="15"/>
-      <c r="I66" s="15"/>
-      <c r="J66" s="15"/>
-      <c r="K66" s="15"/>
-      <c r="L66" s="15"/>
-      <c r="M66" s="15"/>
-      <c r="N66" s="15"/>
-      <c r="O66" s="15"/>
-      <c r="P66" s="15"/>
-      <c r="Q66" s="15"/>
-      <c r="R66" s="15"/>
-      <c r="S66" s="15"/>
-      <c r="T66" s="15"/>
-      <c r="U66" s="15"/>
-      <c r="V66" s="15"/>
-      <c r="W66" s="15"/>
-      <c r="X66" s="15"/>
-      <c r="Y66" s="15"/>
-      <c r="Z66" s="15"/>
-      <c r="AA66" s="15"/>
+      <c r="D65" s="43"/>
+      <c r="E65" s="34"/>
+      <c r="F65" s="34"/>
+      <c r="G65" s="34"/>
+      <c r="H65" s="34"/>
+      <c r="I65" s="34"/>
+      <c r="J65" s="34"/>
+      <c r="K65" s="34"/>
+      <c r="L65" s="34"/>
+      <c r="M65" s="34"/>
+      <c r="N65" s="34"/>
+      <c r="O65" s="34"/>
+      <c r="P65" s="34"/>
+      <c r="Q65" s="34"/>
+      <c r="R65" s="34"/>
+      <c r="S65" s="34"/>
+      <c r="T65" s="34"/>
+      <c r="U65" s="34"/>
+      <c r="V65" s="34"/>
+      <c r="W65" s="34"/>
+      <c r="X65" s="34"/>
+      <c r="Y65" s="34"/>
+      <c r="Z65" s="34"/>
+      <c r="AA65" s="34"/>
+    </row>
+    <row r="66" spans="1:27" s="45" customFormat="1" ht="16">
+      <c r="A66" s="34" t="s">
+        <v>676</v>
+      </c>
+      <c r="B66" s="40" t="s">
+        <v>837</v>
+      </c>
+      <c r="C66" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="D66" s="43"/>
+      <c r="E66" s="34"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="46"/>
+      <c r="I66" s="46"/>
+      <c r="J66" s="46"/>
+      <c r="K66" s="46"/>
+      <c r="L66" s="46"/>
+      <c r="M66" s="46"/>
+      <c r="N66" s="46"/>
+      <c r="O66" s="46"/>
+      <c r="P66" s="46"/>
+      <c r="Q66" s="46"/>
+      <c r="R66" s="46"/>
+      <c r="S66" s="46"/>
+      <c r="T66" s="46"/>
+      <c r="U66" s="46"/>
+      <c r="V66" s="46"/>
+      <c r="W66" s="46"/>
+      <c r="X66" s="46"/>
+      <c r="Y66" s="34"/>
+      <c r="Z66" s="34"/>
+      <c r="AA66" s="34"/>
     </row>
     <row r="67" spans="1:27" ht="16">
-      <c r="A67" s="58" t="s">
-        <v>3784</v>
-      </c>
-      <c r="B67" s="51" t="s">
-        <v>910</v>
-      </c>
-      <c r="C67" s="52" t="s">
-        <v>232</v>
-      </c>
-      <c r="D67" s="53"/>
-      <c r="E67" s="26"/>
+      <c r="A67" s="15"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="25"/>
+      <c r="E67" s="15"/>
       <c r="F67" s="15"/>
       <c r="G67" s="15"/>
       <c r="H67" s="15"/>
@@ -16025,12 +16070,18 @@
       <c r="AA67" s="15"/>
     </row>
     <row r="68" spans="1:27" ht="16">
-      <c r="A68" s="15"/>
-      <c r="B68" s="16"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="25"/>
+      <c r="A68" s="58" t="s">
+        <v>3783</v>
+      </c>
+      <c r="B68" s="51" t="s">
+        <v>869</v>
+      </c>
+      <c r="C68" s="52" t="s">
+        <v>232</v>
+      </c>
+      <c r="D68" s="53"/>
       <c r="E68" s="15"/>
-      <c r="F68" s="15"/>
+      <c r="F68" s="54"/>
       <c r="G68" s="15"/>
       <c r="H68" s="15"/>
       <c r="I68" s="15"/>
@@ -16054,17 +16105,17 @@
       <c r="AA68" s="15"/>
     </row>
     <row r="69" spans="1:27" ht="16">
-      <c r="A69" s="15" t="s">
-        <v>964</v>
-      </c>
-      <c r="B69" s="16" t="s">
-        <v>970</v>
-      </c>
-      <c r="C69" s="17" t="s">
+      <c r="A69" s="58" t="s">
+        <v>3784</v>
+      </c>
+      <c r="B69" s="51" t="s">
+        <v>910</v>
+      </c>
+      <c r="C69" s="52" t="s">
         <v>232</v>
       </c>
-      <c r="D69" s="25"/>
-      <c r="E69" s="15"/>
+      <c r="D69" s="53"/>
+      <c r="E69" s="26"/>
       <c r="F69" s="15"/>
       <c r="G69" s="15"/>
       <c r="H69" s="15"/>
@@ -16089,15 +16140,9 @@
       <c r="AA69" s="15"/>
     </row>
     <row r="70" spans="1:27" ht="16">
-      <c r="A70" s="15" t="s">
-        <v>991</v>
-      </c>
-      <c r="B70" s="16" t="s">
-        <v>998</v>
-      </c>
-      <c r="C70" s="17" t="s">
-        <v>232</v>
-      </c>
+      <c r="A70" s="15"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="17"/>
       <c r="D70" s="25"/>
       <c r="E70" s="15"/>
       <c r="F70" s="15"/>
@@ -16124,9 +16169,15 @@
       <c r="AA70" s="15"/>
     </row>
     <row r="71" spans="1:27" ht="16">
-      <c r="A71" s="15"/>
-      <c r="B71" s="16"/>
-      <c r="C71" s="17"/>
+      <c r="A71" s="15" t="s">
+        <v>964</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>970</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>232</v>
+      </c>
       <c r="D71" s="25"/>
       <c r="E71" s="15"/>
       <c r="F71" s="15"/>
@@ -16154,18 +16205,16 @@
     </row>
     <row r="72" spans="1:27" ht="16">
       <c r="A72" s="15" t="s">
-        <v>964</v>
+        <v>991</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>1012</v>
+        <v>998</v>
       </c>
       <c r="C72" s="17" t="s">
         <v>232</v>
       </c>
       <c r="D72" s="25"/>
-      <c r="E72" s="15" t="s">
-        <v>3798</v>
-      </c>
+      <c r="E72" s="15"/>
       <c r="F72" s="15"/>
       <c r="G72" s="15"/>
       <c r="H72" s="15"/>
@@ -16190,19 +16239,11 @@
       <c r="AA72" s="15"/>
     </row>
     <row r="73" spans="1:27" ht="16">
-      <c r="A73" s="15" t="s">
-        <v>991</v>
-      </c>
-      <c r="B73" s="16" t="s">
-        <v>1019</v>
-      </c>
-      <c r="C73" s="17" t="s">
-        <v>232</v>
-      </c>
+      <c r="A73" s="15"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="17"/>
       <c r="D73" s="25"/>
-      <c r="E73" s="15" t="s">
-        <v>3797</v>
-      </c>
+      <c r="E73" s="15"/>
       <c r="F73" s="15"/>
       <c r="G73" s="15"/>
       <c r="H73" s="15"/>
@@ -16227,11 +16268,19 @@
       <c r="AA73" s="15"/>
     </row>
     <row r="74" spans="1:27" ht="16">
-      <c r="A74" s="15"/>
-      <c r="B74" s="16"/>
-      <c r="C74" s="17"/>
+      <c r="A74" s="15" t="s">
+        <v>964</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C74" s="17" t="s">
+        <v>232</v>
+      </c>
       <c r="D74" s="25"/>
-      <c r="E74" s="15"/>
+      <c r="E74" s="15" t="s">
+        <v>3798</v>
+      </c>
       <c r="F74" s="15"/>
       <c r="G74" s="15"/>
       <c r="H74" s="15"/>
@@ -16257,17 +16306,17 @@
     </row>
     <row r="75" spans="1:27" ht="16">
       <c r="A75" s="15" t="s">
-        <v>964</v>
+        <v>991</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>1029</v>
+        <v>1019</v>
       </c>
       <c r="C75" s="17" t="s">
         <v>232</v>
       </c>
       <c r="D75" s="25"/>
       <c r="E75" s="15" t="s">
-        <v>3800</v>
+        <v>3797</v>
       </c>
       <c r="F75" s="15"/>
       <c r="G75" s="15"/>
@@ -16293,19 +16342,11 @@
       <c r="AA75" s="15"/>
     </row>
     <row r="76" spans="1:27" ht="16">
-      <c r="A76" s="15" t="s">
-        <v>991</v>
-      </c>
-      <c r="B76" s="16" t="s">
-        <v>1032</v>
-      </c>
-      <c r="C76" s="17" t="s">
-        <v>232</v>
-      </c>
+      <c r="A76" s="15"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="17"/>
       <c r="D76" s="25"/>
-      <c r="E76" s="15" t="s">
-        <v>3799</v>
-      </c>
+      <c r="E76" s="15"/>
       <c r="F76" s="15"/>
       <c r="G76" s="15"/>
       <c r="H76" s="15"/>
@@ -16330,11 +16371,19 @@
       <c r="AA76" s="15"/>
     </row>
     <row r="77" spans="1:27" ht="16">
-      <c r="A77" s="15"/>
-      <c r="B77" s="16"/>
-      <c r="C77" s="17"/>
+      <c r="A77" s="15" t="s">
+        <v>964</v>
+      </c>
+      <c r="B77" s="16" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C77" s="17" t="s">
+        <v>232</v>
+      </c>
       <c r="D77" s="25"/>
-      <c r="E77" s="15"/>
+      <c r="E77" s="15" t="s">
+        <v>3800</v>
+      </c>
       <c r="F77" s="15"/>
       <c r="G77" s="15"/>
       <c r="H77" s="15"/>
@@ -16360,16 +16409,18 @@
     </row>
     <row r="78" spans="1:27" ht="16">
       <c r="A78" s="15" t="s">
-        <v>1039</v>
+        <v>991</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>1041</v>
+        <v>1032</v>
       </c>
       <c r="C78" s="17" t="s">
         <v>232</v>
       </c>
       <c r="D78" s="25"/>
-      <c r="E78" s="15"/>
+      <c r="E78" s="15" t="s">
+        <v>3799</v>
+      </c>
       <c r="F78" s="15"/>
       <c r="G78" s="15"/>
       <c r="H78" s="15"/>
@@ -16394,15 +16445,9 @@
       <c r="AA78" s="15"/>
     </row>
     <row r="79" spans="1:27" ht="16">
-      <c r="A79" s="15" t="s">
-        <v>1045</v>
-      </c>
-      <c r="B79" s="16" t="s">
-        <v>1050</v>
-      </c>
-      <c r="C79" s="17" t="s">
-        <v>232</v>
-      </c>
+      <c r="A79" s="15"/>
+      <c r="B79" s="16"/>
+      <c r="C79" s="17"/>
       <c r="D79" s="25"/>
       <c r="E79" s="15"/>
       <c r="F79" s="15"/>
@@ -16429,9 +16474,15 @@
       <c r="AA79" s="15"/>
     </row>
     <row r="80" spans="1:27" ht="16">
-      <c r="A80" s="15"/>
-      <c r="B80" s="16"/>
-      <c r="C80" s="17"/>
+      <c r="A80" s="15" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C80" s="17" t="s">
+        <v>232</v>
+      </c>
       <c r="D80" s="25"/>
       <c r="E80" s="15"/>
       <c r="F80" s="15"/>
@@ -16458,20 +16509,22 @@
       <c r="AA80" s="15"/>
     </row>
     <row r="81" spans="1:27" ht="16">
-      <c r="A81" s="15"/>
+      <c r="A81" s="15" t="s">
+        <v>1045</v>
+      </c>
       <c r="B81" s="16" t="s">
-        <v>1056</v>
-      </c>
-      <c r="C81" s="17"/>
-      <c r="D81" s="60" t="s">
-        <v>3807</v>
-      </c>
-      <c r="E81" s="55"/>
-      <c r="F81" s="55"/>
-      <c r="G81" s="55"/>
-      <c r="H81" s="55"/>
-      <c r="I81" s="56"/>
-      <c r="J81" s="56"/>
+        <v>1050</v>
+      </c>
+      <c r="C81" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="D81" s="25"/>
+      <c r="E81" s="15"/>
+      <c r="F81" s="15"/>
+      <c r="G81" s="15"/>
+      <c r="H81" s="15"/>
+      <c r="I81" s="15"/>
+      <c r="J81" s="15"/>
       <c r="K81" s="15"/>
       <c r="L81" s="15"/>
       <c r="M81" s="15"/>
@@ -16490,48 +16543,93 @@
       <c r="Z81" s="15"/>
       <c r="AA81" s="15"/>
     </row>
-    <row r="82" spans="1:27" ht="15.75" customHeight="1"/>
-    <row r="83" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A83" s="63" t="s">
-        <v>3818</v>
-      </c>
-      <c r="B83" s="61" t="s">
-        <v>3811</v>
-      </c>
-      <c r="C83" s="61" t="s">
-        <v>65</v>
-      </c>
-      <c r="E83" s="62" t="s">
-        <v>3741</v>
-      </c>
-    </row>
-    <row r="84" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A84" s="63" t="s">
-        <v>3818</v>
-      </c>
-      <c r="B84" s="61" t="s">
-        <v>3812</v>
-      </c>
-      <c r="C84" s="61" t="s">
-        <v>360</v>
-      </c>
-      <c r="E84" s="62"/>
-    </row>
+    <row r="82" spans="1:27" ht="16">
+      <c r="A82" s="15"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="17"/>
+      <c r="D82" s="25"/>
+      <c r="E82" s="15"/>
+      <c r="F82" s="15"/>
+      <c r="G82" s="15"/>
+      <c r="H82" s="15"/>
+      <c r="I82" s="15"/>
+      <c r="J82" s="15"/>
+      <c r="K82" s="15"/>
+      <c r="L82" s="15"/>
+      <c r="M82" s="15"/>
+      <c r="N82" s="15"/>
+      <c r="O82" s="15"/>
+      <c r="P82" s="15"/>
+      <c r="Q82" s="15"/>
+      <c r="R82" s="15"/>
+      <c r="S82" s="15"/>
+      <c r="T82" s="15"/>
+      <c r="U82" s="15"/>
+      <c r="V82" s="15"/>
+      <c r="W82" s="15"/>
+      <c r="X82" s="15"/>
+      <c r="Y82" s="15"/>
+      <c r="Z82" s="15"/>
+      <c r="AA82" s="15"/>
+    </row>
+    <row r="83" spans="1:27" ht="16">
+      <c r="A83" s="15"/>
+      <c r="B83" s="16" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C83" s="17"/>
+      <c r="D83" s="60" t="s">
+        <v>3807</v>
+      </c>
+      <c r="E83" s="55"/>
+      <c r="F83" s="55"/>
+      <c r="G83" s="55"/>
+      <c r="H83" s="55"/>
+      <c r="I83" s="56"/>
+      <c r="J83" s="56"/>
+      <c r="K83" s="15"/>
+      <c r="L83" s="15"/>
+      <c r="M83" s="15"/>
+      <c r="N83" s="15"/>
+      <c r="O83" s="15"/>
+      <c r="P83" s="15"/>
+      <c r="Q83" s="15"/>
+      <c r="R83" s="15"/>
+      <c r="S83" s="15"/>
+      <c r="T83" s="15"/>
+      <c r="U83" s="15"/>
+      <c r="V83" s="15"/>
+      <c r="W83" s="15"/>
+      <c r="X83" s="15"/>
+      <c r="Y83" s="15"/>
+      <c r="Z83" s="15"/>
+      <c r="AA83" s="15"/>
+    </row>
+    <row r="84" spans="1:27" ht="15.75" customHeight="1"/>
     <row r="85" spans="1:27" ht="15.75" customHeight="1">
       <c r="A85" s="63" t="s">
         <v>3818</v>
       </c>
       <c r="B85" s="61" t="s">
-        <v>3813</v>
+        <v>3811</v>
       </c>
       <c r="C85" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="E85" s="62" t="s">
+        <v>3741</v>
+      </c>
+    </row>
+    <row r="86" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A86" s="63" t="s">
+        <v>3818</v>
+      </c>
+      <c r="B86" s="61" t="s">
+        <v>3812</v>
+      </c>
+      <c r="C86" s="61" t="s">
         <v>360</v>
       </c>
-      <c r="E85" s="62"/>
-    </row>
-    <row r="86" spans="1:27" ht="15.75" customHeight="1">
-      <c r="B86" s="61"/>
-      <c r="C86" s="61"/>
       <c r="E86" s="62"/>
     </row>
     <row r="87" spans="1:27" ht="15.75" customHeight="1">
@@ -16539,45 +16637,60 @@
         <v>3818</v>
       </c>
       <c r="B87" s="61" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="C87" s="61" t="s">
-        <v>65</v>
-      </c>
-      <c r="E87" s="62" t="s">
-        <v>3746</v>
-      </c>
+        <v>360</v>
+      </c>
+      <c r="E87" s="62"/>
     </row>
     <row r="88" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A88" s="63" t="s">
-        <v>3818</v>
-      </c>
-      <c r="B88" s="61" t="s">
-        <v>3815</v>
-      </c>
-      <c r="C88" s="61" t="s">
-        <v>360</v>
-      </c>
-      <c r="E88" s="62" t="s">
-        <v>3816</v>
-      </c>
+      <c r="B88" s="61"/>
+      <c r="C88" s="61"/>
+      <c r="E88" s="62"/>
     </row>
     <row r="89" spans="1:27" ht="15.75" customHeight="1">
       <c r="A89" s="63" t="s">
         <v>3818</v>
       </c>
       <c r="B89" s="61" t="s">
+        <v>3814</v>
+      </c>
+      <c r="C89" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="E89" s="62" t="s">
+        <v>3746</v>
+      </c>
+    </row>
+    <row r="90" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A90" s="63" t="s">
+        <v>3818</v>
+      </c>
+      <c r="B90" s="61" t="s">
+        <v>3815</v>
+      </c>
+      <c r="C90" s="61" t="s">
+        <v>360</v>
+      </c>
+      <c r="E90" s="62" t="s">
+        <v>3816</v>
+      </c>
+    </row>
+    <row r="91" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A91" s="63" t="s">
+        <v>3818</v>
+      </c>
+      <c r="B91" s="61" t="s">
         <v>3817</v>
       </c>
-      <c r="C89" s="61" t="s">
+      <c r="C91" s="61" t="s">
         <v>360</v>
       </c>
-      <c r="E89" s="62">
+      <c r="E91" s="62">
         <v>2018</v>
       </c>
     </row>
-    <row r="90" spans="1:27" ht="15.75" customHeight="1"/>
-    <row r="91" spans="1:27" ht="15.75" customHeight="1"/>
     <row r="92" spans="1:27" ht="15.75" customHeight="1"/>
     <row r="93" spans="1:27" ht="15.75" customHeight="1"/>
     <row r="94" spans="1:27" ht="15.75" customHeight="1"/>
@@ -17494,14 +17607,16 @@
     <row r="1005" ht="15.75" customHeight="1"/>
     <row r="1006" ht="15.75" customHeight="1"/>
     <row r="1007" ht="15.75" customHeight="1"/>
+    <row r="1008" ht="15.75" customHeight="1"/>
+    <row r="1009" ht="15.75" customHeight="1"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="TEI Publication date" prompt="The year this metadata document will be marked a published; e.g., 2018, 2019, etc. _x000a__x000a_NOT the year of the book's publication." sqref="B13" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E27" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E29" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E22" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E29" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E31" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E23" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>